<commit_message>
add mapping and edf validations
</commit_message>
<xml_diff>
--- a/workspace/gradient_fp_validation/gradient_fp_validation_times.xlsx
+++ b/workspace/gradient_fp_validation/gradient_fp_validation_times.xlsx
@@ -465,19 +465,19 @@
         <v>0.5</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0005191483028465882</v>
+        <v>0.0005255733983358369</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0006912733154604212</v>
+        <v>0.0006956399435875938</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0002339240990113467</v>
+        <v>0.0002342874786700122</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0001730884407879785</v>
+        <v>0.0001725392614025623</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0001749175606528297</v>
+        <v>0.0001745209208456799</v>
       </c>
     </row>
     <row r="3">
@@ -485,19 +485,19 @@
         <v>0.5210526315789473</v>
       </c>
       <c r="B3" t="n">
-        <v>0.00054059921822045</v>
+        <v>0.0005465241411002353</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0007240567775443197</v>
+        <v>0.0007245875801891088</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0002452465999522246</v>
+        <v>0.0002455608404125087</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0001729357810108923</v>
+        <v>0.0001735049794660881</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0001793316393741406</v>
+        <v>0.000179678279964719</v>
       </c>
     </row>
     <row r="4">
@@ -505,19 +505,19 @@
         <v>0.5421052631578948</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0005527517013251781</v>
+        <v>0.0006106475047999993</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0007366607658332214</v>
+        <v>0.0008222499751718715</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0002505349204875529</v>
+        <v>0.0002710141602437943</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0001754308197996579</v>
+        <v>0.0001838725194102153</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0001800901218666695</v>
+        <v>0.0001960533406236209</v>
       </c>
     </row>
     <row r="5">
@@ -525,19 +525,19 @@
         <v>0.5631578947368421</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0005952083953889086</v>
+        <v>0.00061323837202508</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0008263166400138288</v>
+        <v>0.0007727684028213844</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0002737257786793634</v>
+        <v>0.0002616132993716746</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0001900341402506456</v>
+        <v>0.0001832933802506886</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0001922567008296028</v>
+        <v>0.0001839850610122084</v>
       </c>
     </row>
     <row r="6">
@@ -545,19 +545,19 @@
         <v>0.5842105263157895</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0006624250463210047</v>
+        <v>0.0006715451017953455</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0008283099991967901</v>
+        <v>0.0008236432867124677</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0002786216817912646</v>
+        <v>0.0002725849786656909</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0001869674597401172</v>
+        <v>0.0001856482806033455</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0001936808199388906</v>
+        <v>0.0001917849620804191</v>
       </c>
     </row>
     <row r="7">
@@ -565,19 +565,19 @@
         <v>0.6052631578947368</v>
       </c>
       <c r="B7" t="n">
-        <v>0.001416512536816299</v>
+        <v>0.001330756686511449</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0008943651238223538</v>
+        <v>0.0008985550364013762</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0002994833007687703</v>
+        <v>0.0002851666577043943</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0001988891389919445</v>
+        <v>0.0001917608804069459</v>
       </c>
       <c r="F7" t="n">
-        <v>0.000211771740578115</v>
+        <v>0.0002058649994432926</v>
       </c>
     </row>
     <row r="8">
@@ -585,19 +585,19 @@
         <v>0.6263157894736842</v>
       </c>
       <c r="B8" t="n">
-        <v>0.001350355004542507</v>
+        <v>0.001419190007727593</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0009645225433632731</v>
+        <v>0.001108905853470787</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0003274816629709676</v>
+        <v>0.0002974100204301067</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0002012908406322822</v>
+        <v>0.0001931234402582049</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0002149366430239752</v>
+        <v>0.0002109799810568802</v>
       </c>
     </row>
     <row r="9">
@@ -605,19 +605,19 @@
         <v>0.6473684210526316</v>
       </c>
       <c r="B9" t="n">
-        <v>0.001779325051466003</v>
+        <v>0.002052134192781523</v>
       </c>
       <c r="C9" t="n">
-        <v>0.001253805846208707</v>
+        <v>0.001174770799116231</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0003928566831746139</v>
+        <v>0.0002951232623308897</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0002241057206992991</v>
+        <v>0.000191466678516008</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0002341916403383948</v>
+        <v>0.0002127883594948799</v>
       </c>
     </row>
     <row r="10">
@@ -625,19 +625,19 @@
         <v>0.6684210526315789</v>
       </c>
       <c r="B10" t="n">
-        <v>0.00239916670077946</v>
+        <v>0.002096100819180719</v>
       </c>
       <c r="C10" t="n">
-        <v>0.001272420000750571</v>
+        <v>0.001161795758525841</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0003990733611863106</v>
+        <v>0.0002915658225538209</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0002375107805710286</v>
+        <v>0.0002108740992844105</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0002359574820729904</v>
+        <v>0.0002049824403366074</v>
       </c>
     </row>
     <row r="11">
@@ -645,19 +645,19 @@
         <v>0.6894736842105263</v>
       </c>
       <c r="B11" t="n">
-        <v>0.003364795834640973</v>
+        <v>0.0035353924613446</v>
       </c>
       <c r="C11" t="n">
-        <v>0.001479785885894671</v>
+        <v>0.001484045895631425</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0004763081815326586</v>
+        <v>0.0003117833018768579</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0002590350402169861</v>
+        <v>0.0002032782990136184</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0002623083611251786</v>
+        <v>0.0002127017205930315</v>
       </c>
     </row>
     <row r="12">
@@ -665,19 +665,19 @@
         <v>0.7105263157894737</v>
       </c>
       <c r="B12" t="n">
-        <v>0.007410586654441431</v>
+        <v>0.007560601613367908</v>
       </c>
       <c r="C12" t="n">
-        <v>0.003429287488106638</v>
+        <v>0.003513533374061808</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0006184533625491895</v>
+        <v>0.0002853217202937231</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0002944783589919097</v>
+        <v>0.0002001441601896659</v>
       </c>
       <c r="F12" t="n">
-        <v>0.000293170782388188</v>
+        <v>0.0002207475615432486</v>
       </c>
     </row>
     <row r="13">
@@ -685,19 +685,19 @@
         <v>0.7315789473684211</v>
       </c>
       <c r="B13" t="n">
-        <v>0.01606169518141541</v>
+        <v>0.01639937072061002</v>
       </c>
       <c r="C13" t="n">
-        <v>0.005594409935874864</v>
+        <v>0.005661338327918201</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0007638600398786366</v>
+        <v>0.0002906525204889476</v>
       </c>
       <c r="E13" t="n">
-        <v>0.00031243916018866</v>
+        <v>0.0002057909205905162</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0003162400203291327</v>
+        <v>0.0002181617222959176</v>
       </c>
     </row>
     <row r="14">
@@ -705,19 +705,19 @@
         <v>0.7526315789473684</v>
       </c>
       <c r="B14" t="n">
-        <v>0.02326163815043401</v>
+        <v>0.02277728251414373</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01030554989003576</v>
+        <v>0.009765807497315109</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0009785950125660748</v>
+        <v>0.0003348342009121552</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0003698892600368708</v>
+        <v>0.0002080366795416921</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0003721732975100167</v>
+        <v>0.0002442875411361456</v>
       </c>
     </row>
     <row r="15">
@@ -725,19 +725,19 @@
         <v>0.7736842105263158</v>
       </c>
       <c r="B15" t="n">
-        <v>0.03790118152508512</v>
+        <v>0.03828838171204552</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01936075660283677</v>
+        <v>0.01963164651591796</v>
       </c>
       <c r="D15" t="n">
-        <v>0.001683724167232867</v>
+        <v>0.0003139883774565533</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0004063283398863859</v>
+        <v>0.0001707467384403571</v>
       </c>
       <c r="F15" t="n">
-        <v>0.000449889978626743</v>
+        <v>0.0001789108195225708</v>
       </c>
     </row>
     <row r="16">
@@ -745,19 +745,19 @@
         <v>0.7947368421052632</v>
       </c>
       <c r="B16" t="n">
-        <v>0.07542231110157445</v>
+        <v>0.07465762879641261</v>
       </c>
       <c r="C16" t="n">
-        <v>0.03158523064688779</v>
+        <v>0.03163599542807788</v>
       </c>
       <c r="D16" t="n">
-        <v>0.002336232411325909</v>
+        <v>0.000248636600736063</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0004425782567705028</v>
+        <v>0.000139395019505173</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0004543883260339499</v>
+        <v>0.0001567224599421024</v>
       </c>
     </row>
     <row r="17">
@@ -765,19 +765,19 @@
         <v>0.8157894736842105</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1048002022749279</v>
+        <v>0.1053145892790053</v>
       </c>
       <c r="C17" t="n">
-        <v>0.04824298810912296</v>
+        <v>0.04680061661754735</v>
       </c>
       <c r="D17" t="n">
-        <v>0.002704903292178642</v>
+        <v>0.0002727658793446608</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0005450707624549977</v>
+        <v>0.0001478707807837054</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0004917391200433486</v>
+        <v>0.0001438408193644136</v>
       </c>
     </row>
     <row r="18">
@@ -785,19 +785,19 @@
         <v>0.8368421052631578</v>
       </c>
       <c r="B18" t="n">
-        <v>0.15749180032406</v>
+        <v>0.1553878969780635</v>
       </c>
       <c r="C18" t="n">
-        <v>0.05911674973554909</v>
+        <v>0.06007049338310026</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00413128005573526</v>
+        <v>0.0002565907582174987</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0006600916993920691</v>
+        <v>0.0001459799610893242</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0006101674580713734</v>
+        <v>0.000165651701099705</v>
       </c>
     </row>
     <row r="19">
@@ -805,19 +805,19 @@
         <v>0.8578947368421053</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2119102615898009</v>
+        <v>0.2137059942859924</v>
       </c>
       <c r="C19" t="n">
-        <v>0.08057446950930171</v>
+        <v>0.08185323432320729</v>
       </c>
       <c r="D19" t="n">
-        <v>0.004589249957352877</v>
+        <v>0.0002343049211776815</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0007397383023635485</v>
+        <v>0.0001243582618189976</v>
       </c>
       <c r="F19" t="n">
-        <v>0.000748875041899737</v>
+        <v>0.0001344591812812723</v>
       </c>
     </row>
     <row r="20">
@@ -825,19 +825,19 @@
         <v>0.8789473684210527</v>
       </c>
       <c r="B20" t="n">
-        <v>0.3692922527430346</v>
+        <v>0.3651776934834197</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1211676936701406</v>
+        <v>0.1190055196243338</v>
       </c>
       <c r="D20" t="n">
-        <v>0.004484922475239727</v>
+        <v>0.0002027933002682403</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0007552491192473099</v>
+        <v>0.0001061716198455542</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0008435032051056624</v>
+        <v>0.0001485299412161112</v>
       </c>
     </row>
     <row r="21">
@@ -845,19 +845,19 @@
         <v>0.9</v>
       </c>
       <c r="B21" t="n">
-        <v>0.5227211336721667</v>
+        <v>0.5197520854510367</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1629596122645307</v>
+        <v>0.1618393243907485</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0063645525125321</v>
+        <v>0.0002756824588868767</v>
       </c>
       <c r="E21" t="n">
-        <v>0.001156547578284517</v>
+        <v>0.0001215233988477848</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0010986258671619</v>
+        <v>0.0001584417390404269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>